<commit_message>
add my own tache
</commit_message>
<xml_diff>
--- a/Stage/Stagiaires/Nya-Youssef.xlsx
+++ b/Stage/Stagiaires/Nya-Youssef.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="12240" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>Tâche</t>
   </si>
@@ -32,12 +32,93 @@
   </si>
   <si>
     <t>Date Fin</t>
+  </si>
+  <si>
+    <t>Analyse fonctionelle</t>
+  </si>
+  <si>
+    <t>Vtts-windows-app</t>
+  </si>
+  <si>
+    <t>Diagramme ca utilisation Securitie gwin</t>
+  </si>
+  <si>
+    <t>Diagramme cas utilisation Securitie pour  Gwin</t>
+  </si>
+  <si>
+    <t>Sport-club-management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagramme de classe  </t>
+  </si>
+  <si>
+    <t>Diagramme de classz de sport clob management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réalisation </t>
+  </si>
+  <si>
+    <t>Add All class to project c#</t>
+  </si>
+  <si>
+    <t>Ajouter tous les class au projet avec c#</t>
+  </si>
+  <si>
+    <t>Securitie</t>
+  </si>
+  <si>
+    <t>ajouter permission au utilisateur concerné</t>
+  </si>
+  <si>
+    <t>compléter la tradiction des propriétés</t>
+  </si>
+  <si>
+    <t>compléter la tradiction des propriétés dans une fichier XL</t>
+  </si>
+  <si>
+    <t>Modifier les type string</t>
+  </si>
+  <si>
+    <t>modifier tous les variable de type string en type LocalizedString</t>
+  </si>
+  <si>
+    <t>Formation</t>
+  </si>
+  <si>
+    <t>formation sur github</t>
+  </si>
+  <si>
+    <t>informer stagiaire sur github</t>
+  </si>
+  <si>
+    <t>REALISATION</t>
+  </si>
+  <si>
+    <t>Ajouter des autorisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajouter autorisation pour  utilisateur admin </t>
+  </si>
+  <si>
+    <t>Realisation</t>
+  </si>
+  <si>
+    <t>ajouter les type des specialities</t>
+  </si>
+  <si>
+    <t>ajouter les types des specialitie par defeaut</t>
+  </si>
+  <si>
+    <t>dimonstration vedio github</t>
+  </si>
+  <si>
+    <t>dimonstration vedio Pour expliquer comment la facon de update projet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -135,7 +216,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -210,6 +291,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -245,6 +343,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -424,10 +539,10 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A2" sqref="A2:F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="28.140625" customWidth="1"/>
@@ -457,58 +572,225 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2">
+        <v>42863</v>
+      </c>
+      <c r="F2" s="2">
+        <v>42863</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2">
+        <v>42853</v>
+      </c>
+      <c r="F3" s="2">
+        <v>42853</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2">
+        <v>42857</v>
+      </c>
+      <c r="F4" s="2">
+        <v>42858</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2">
+        <v>42857</v>
+      </c>
+      <c r="F5" s="2">
+        <v>42857</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2">
+        <v>42850</v>
+      </c>
+      <c r="F6" s="2">
+        <v>42850</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2">
+        <v>42860</v>
+      </c>
+      <c r="F7" s="2">
+        <v>42860</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="2">
+        <v>42857</v>
+      </c>
+      <c r="F8" s="2">
+        <v>42857</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="2">
+        <v>42859</v>
+      </c>
+      <c r="F9" s="2">
+        <v>42859</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="2">
+        <v>42863</v>
+      </c>
+      <c r="F10" s="2">
+        <v>42863</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="2">
+        <v>42863</v>
+      </c>
+      <c r="F11" s="2">
+        <v>42863</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="2">
+        <v>42863</v>
+      </c>
+      <c r="F12" s="2">
+        <v>42863</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>

</xml_diff>